<commit_message>
atualizacao na logica de decodificacao do caractere predito
</commit_message>
<xml_diff>
--- a/dados/caracteres-limpo.xlsx
+++ b/dados/caracteres-limpo.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
feat: adicionado treino com validacao
</commit_message>
<xml_diff>
--- a/dados/caracteres-limpo.xlsx
+++ b/dados/caracteres-limpo.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -736,52 +736,52 @@
       </c>
       <c r="BI1" s="1" t="inlineStr">
         <is>
-          <t>atributo60</t>
+          <t>rotulo0</t>
         </is>
       </c>
       <c r="BJ1" s="1" t="inlineStr">
         <is>
-          <t>atributo61</t>
+          <t>rotulo1</t>
         </is>
       </c>
       <c r="BK1" s="1" t="inlineStr">
         <is>
-          <t>atributo62</t>
+          <t>rotulo2</t>
         </is>
       </c>
       <c r="BL1" s="1" t="inlineStr">
         <is>
-          <t>rotulo0</t>
+          <t>rotulo3</t>
         </is>
       </c>
       <c r="BM1" s="1" t="inlineStr">
         <is>
-          <t>rotulo1</t>
+          <t>rotulo4</t>
         </is>
       </c>
       <c r="BN1" s="1" t="inlineStr">
         <is>
-          <t>rotulo2</t>
+          <t>rotulo5</t>
         </is>
       </c>
       <c r="BO1" s="1" t="inlineStr">
         <is>
-          <t>rotulo3</t>
+          <t>rotulo6</t>
         </is>
       </c>
       <c r="BP1" s="1" t="inlineStr">
         <is>
-          <t>rotulo4</t>
+          <t>rotulo7</t>
         </is>
       </c>
       <c r="BQ1" s="1" t="inlineStr">
         <is>
-          <t>rotulo5</t>
+          <t>rotulo8</t>
         </is>
       </c>
       <c r="BR1" s="1" t="inlineStr">
         <is>
-          <t>rotulo6</t>
+          <t>rotulo9</t>
         </is>
       </c>
     </row>

</xml_diff>